<commit_message>
Search Data and Select Data in Dropdown
</commit_message>
<xml_diff>
--- a/KeywordDrivenFramework/Sheets/Keyworddriven.xlsx
+++ b/KeywordDrivenFramework/Sheets/Keyworddriven.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\KeywordDriven\KeywordDrivenFramework\Sheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="13350" windowHeight="6600"/>
   </bookViews>
@@ -108,7 +113,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,6 +154,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -197,7 +205,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -232,7 +240,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -444,7 +452,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Excel Sheet Final Changes
</commit_message>
<xml_diff>
--- a/KeywordDrivenFramework/Sheets/Keyworddriven.xlsx
+++ b/KeywordDrivenFramework/Sheets/Keyworddriven.xlsx
@@ -117,24 +117,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>name=username</t>
-  </si>
-  <si>
-    <t>name=password</t>
-  </si>
-  <si>
-    <t>xpath=//*[@id=\"app\"]/div[1]/div/div[1]/div/div[2]/div[2]/form/div[3]/button</t>
-  </si>
-  <si>
-    <t>xpath=//*[@id=\"app\"]/div[1]/div[1]/aside/nav/div[2]/ul/li[9]/a</t>
-  </si>
-  <si>
-    <t>xpath=//*[@id=\"app\"]/div[1]/div[2]/div[2]/div/div[1]/div[2]/form/div[1]/div/div[2]/div/div[2]/div/div/div[1]</t>
-  </si>
-  <si>
-    <t>xpath=//*[@id=\"app\"]/div[1]/div[2]/div[2]/div/div[1]/div[2]/form/div[2]/button[2]</t>
-  </si>
-  <si>
     <t>chrome</t>
   </si>
   <si>
@@ -145,6 +127,24 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>name :username</t>
+  </si>
+  <si>
+    <t>name :password</t>
+  </si>
+  <si>
+    <t>xpath ://*[@id="app"]/div[1]/div/div[1]/div/div[2]/div[2]/form/div[3]/button</t>
+  </si>
+  <si>
+    <t>xpath ://*[@id=\"app\"]/div[1]/div[1]/aside/nav/div[2]/ul/li[9]/a</t>
+  </si>
+  <si>
+    <t>xpath ://*[@id=\"app\"]/div[1]/div[2]/div[2]/div/div[1]/div[2]/form/div[1]/div/div[2]/div/div[2]/div/div/div[1]</t>
+  </si>
+  <si>
+    <t>xpath ://*[@id=\"app\"]/div[1]/div[2]/div[2]/div/div[1]/div[2]/form/div[2]/button[2]</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +508,7 @@
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="78.28515625" customWidth="1"/>
+    <col min="4" max="4" width="102.7109375" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="38.42578125" customWidth="1"/>
   </cols>
@@ -550,7 +550,7 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -570,7 +570,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -584,13 +584,13 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -604,13 +604,13 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -624,7 +624,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -644,7 +644,7 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
         <v>26</v>
@@ -664,7 +664,7 @@
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
@@ -684,7 +684,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Excel Sheet Changes One
</commit_message>
<xml_diff>
--- a/KeywordDrivenFramework/Sheets/Keyworddriven.xlsx
+++ b/KeywordDrivenFramework/Sheets/Keyworddriven.xlsx
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +510,7 @@
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="102.7109375" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="38.42578125" customWidth="1"/>
+    <col min="6" max="6" width="66.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>